<commit_message>
Sprint Commit Day 10
</commit_message>
<xml_diff>
--- a/Written Tasks/GotoGro WBS.xlsx
+++ b/Written Tasks/GotoGro WBS.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jarvi\Desktop\Managing Software\msp-gotogro\Written Tasks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{831F6CBE-E062-421F-A465-67F57721AA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDC11CE9-E1B6-4B00-BD18-75696987E936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CE9BC19B-72E2-48A1-B107-A8840272799F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Sprint 1'!$A$1:$I$44</definedName>
@@ -769,7 +770,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,4 +1650,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2997EC8E-0F95-42CB-8CEE-4E882F032190}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>